<commit_message>
mass error for all suspects done
</commit_message>
<xml_diff>
--- a/data/Sus. + ms2 data.xlsx
+++ b/data/Sus. + ms2 data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PFAS project\Data\Suspect Screening\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD6986E-49BD-46BA-9681-462E6A40EDFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99D7439-53E2-40D4-9C1C-64C2B173ACDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="5790" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3896" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3900" uniqueCount="466">
   <si>
     <t>10_2 FTSA</t>
   </si>
@@ -1423,6 +1423,9 @@
   </si>
   <si>
     <t>HPFO-DA-br</t>
+  </si>
+  <si>
+    <t>ND</t>
   </si>
 </sst>
 </file>
@@ -1888,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM47"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+    <sheetView topLeftCell="AU1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BD5" sqref="BD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18865,9 +18868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18883,9 +18886,9 @@
     <col min="9" max="9" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -18977,7 +18980,7 @@
         <v>590.98748499999999</v>
       </c>
       <c r="E2">
-        <f>(D2-F2)/F2*10^6</f>
+        <f t="shared" ref="E2:E9" si="0">(D2-F2)/F2*10^6</f>
         <v>-0.18274495308178135</v>
       </c>
       <c r="F2">
@@ -19036,7 +19039,7 @@
         <v>640.98490000000004</v>
       </c>
       <c r="E3">
-        <f>(D3-F3)/F3*10^6</f>
+        <f t="shared" si="0"/>
         <v>0.78317038846728215</v>
       </c>
       <c r="F3">
@@ -19078,7 +19081,7 @@
         <v>241.01009999999999</v>
       </c>
       <c r="E4">
-        <f>(D4-F4)/F4*10^6</f>
+        <f t="shared" si="0"/>
         <v>0.98336224521437299</v>
       </c>
       <c r="F4">
@@ -19120,7 +19123,7 @@
         <v>341.00336499999997</v>
       </c>
       <c r="E5">
-        <f>(D5-F5)/F5*10^6</f>
+        <f t="shared" si="0"/>
         <v>-0.57184153742929578</v>
       </c>
       <c r="F5">
@@ -19164,7 +19167,7 @@
         <v>391.00110000000001</v>
       </c>
       <c r="E6">
-        <f>(D6-F6)/F6*10^6</f>
+        <f t="shared" si="0"/>
         <v>1.8695634530980079</v>
       </c>
       <c r="F6">
@@ -19181,6 +19184,16 @@
       </c>
       <c r="K6" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="L6" s="15">
+        <v>4.41</v>
+      </c>
+      <c r="M6">
+        <v>391.21282000000002</v>
+      </c>
+      <c r="N6">
+        <f>(F6-M6)/M6*10^6</f>
+        <v>-543.05735686280445</v>
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -19206,7 +19219,7 @@
         <v>440.997075</v>
       </c>
       <c r="E7">
-        <f>(D7-F7)/F7*10^6</f>
+        <f t="shared" si="0"/>
         <v>-0.22675882215095358</v>
       </c>
       <c r="F7">
@@ -19283,7 +19296,7 @@
         <v>490.99400499999996</v>
       </c>
       <c r="E8">
-        <f>(D8-F8)/F8*10^6</f>
+        <f t="shared" si="0"/>
         <v>4.8880436268014547E-2</v>
       </c>
       <c r="F8">
@@ -19335,7 +19348,7 @@
         <v>540.99066499999992</v>
       </c>
       <c r="E9">
-        <f>(D9-F9)/F9*10^6</f>
+        <f t="shared" si="0"/>
         <v>-0.2255121583670151</v>
       </c>
       <c r="F9">
@@ -19411,7 +19424,7 @@
         <v>626.95468499999993</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E2:E20" si="0">(D10-F10)/F10*10^6</f>
+        <f t="shared" ref="E10:E20" si="1">(D10-F10)/F10*10^6</f>
         <v>0.16747624678373699</v>
       </c>
       <c r="F10">
@@ -19497,7 +19510,7 @@
         <v>726.94960000000003</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9368642986914817</v>
       </c>
       <c r="F11">
@@ -19514,6 +19527,13 @@
       </c>
       <c r="K11" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="M11">
+        <v>726.94929999999999</v>
+      </c>
+      <c r="N11">
+        <f>(F11-M11)/M11*10^6</f>
+        <v>-1.5241778209907346</v>
       </c>
       <c r="W11" s="11" t="s">
         <v>364</v>
@@ -19541,7 +19561,7 @@
         <v>426.96780000000001</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0398921457964485</v>
       </c>
       <c r="F12">
@@ -19602,7 +19622,7 @@
         <v>526.96159999999998</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1993298144920082</v>
       </c>
       <c r="F13">
@@ -19619,6 +19639,13 @@
       </c>
       <c r="K13" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="M13">
+        <v>526.96173999999996</v>
+      </c>
+      <c r="N13">
+        <f>(F13-M13)/M13*10^6</f>
+        <v>-1.4650019942312389</v>
       </c>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -19707,7 +19734,7 @@
         <v>528.95479999999998</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.75242780571155576</v>
       </c>
       <c r="F16">
@@ -19721,6 +19748,13 @@
       </c>
       <c r="K16" s="8" t="s">
         <v>186</v>
+      </c>
+      <c r="M16">
+        <v>528.93074000000001</v>
+      </c>
+      <c r="N16">
+        <f>(F16-M16)/M16*10^6</f>
+        <v>44.73553569593021</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
@@ -19737,7 +19771,7 @@
         <v>578.95209999999997</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5407170547291671</v>
       </c>
       <c r="F17">
@@ -19764,7 +19798,7 @@
         <v>428.9615</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6551629346505348</v>
       </c>
       <c r="F18">
@@ -19816,7 +19850,7 @@
         <v>478.95800000000003</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84349847133444988</v>
       </c>
       <c r="F19">
@@ -19843,7 +19877,7 @@
         <v>560.92650000000003</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6351886126243254E-2</v>
       </c>
       <c r="F20">
@@ -20032,7 +20066,7 @@
         <v>460.932705</v>
       </c>
       <c r="E25">
-        <f t="shared" ref="E25:E41" si="1">(D25-F25)/F25*10^6</f>
+        <f t="shared" ref="E25:E41" si="2">(D25-F25)/F25*10^6</f>
         <v>-0.34061359678346614</v>
       </c>
       <c r="F25">
@@ -20055,6 +20089,10 @@
       </c>
       <c r="M25">
         <v>462.96359999999999</v>
+      </c>
+      <c r="N25">
+        <f>(F25-M25)/M25*10^6</f>
+        <v>-4386.3880443300195</v>
       </c>
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
@@ -20085,7 +20123,7 @@
         <v>510.9307</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0198474753852969</v>
       </c>
       <c r="F26">
@@ -20126,7 +20164,7 @@
         <v>414.93150000000003</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2749108574704235</v>
       </c>
       <c r="F27">
@@ -20140,6 +20178,9 @@
       </c>
       <c r="K27" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="M27" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -20156,7 +20197,7 @@
         <v>464.92809999999997</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.69473156038235861</v>
       </c>
       <c r="F28">
@@ -20170,6 +20211,16 @@
       </c>
       <c r="K28" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="L28" s="15">
+        <v>4.51</v>
+      </c>
+      <c r="M28">
+        <v>464.24754999999999</v>
+      </c>
+      <c r="N28">
+        <f>(F28-M28)/M28*10^6</f>
+        <v>1465.2247491666938</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
@@ -20186,7 +20237,7 @@
         <v>514.92489999999998</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.61562413304990682</v>
       </c>
       <c r="F29">
@@ -20235,7 +20286,7 @@
         <v>564.92179999999996</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.72753485350066338</v>
       </c>
       <c r="F30">
@@ -20262,7 +20313,7 @@
         <v>576.92160000000001</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34666767442407709</v>
       </c>
       <c r="F31">
@@ -20276,6 +20327,9 @@
       </c>
       <c r="K31" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="M31" t="s">
+        <v>465</v>
       </c>
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
@@ -20306,7 +20360,7 @@
         <v>626.91930000000002</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7546148764941552</v>
       </c>
       <c r="F32">
@@ -20333,7 +20387,7 @@
         <v>426.93090000000001</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.23422988720635876</v>
       </c>
       <c r="F33">
@@ -20360,7 +20414,7 @@
         <v>476.9282</v>
       </c>
       <c r="E34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.88692674323318488</v>
       </c>
       <c r="F34">
@@ -20374,6 +20428,9 @@
       </c>
       <c r="K34" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="M34" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
@@ -20390,7 +20447,7 @@
         <v>526.92520000000002</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1709455583207065</v>
       </c>
       <c r="F35">
@@ -20407,6 +20464,9 @@
       </c>
       <c r="L35" s="23" t="s">
         <v>336</v>
+      </c>
+      <c r="M35" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
@@ -20423,7 +20483,7 @@
         <v>548.00140499999998</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2354009117587654</v>
       </c>
       <c r="F36">
@@ -20437,6 +20497,16 @@
       </c>
       <c r="K36" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="L36" s="15">
+        <v>4.37</v>
+      </c>
+      <c r="M36">
+        <v>548.00219000000004</v>
+      </c>
+      <c r="N36">
+        <f>(F36-M36)/M36*10^6</f>
+        <v>-1.6678765464053991</v>
       </c>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
@@ -20462,7 +20532,7 @@
         <v>597.99819500000001</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18896381687017344</v>
       </c>
       <c r="F37">
@@ -20529,7 +20599,7 @@
         <v>647.99515499999995</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.412040287589446</v>
       </c>
       <c r="F38">
@@ -20543,6 +20613,16 @@
       </c>
       <c r="K38" s="8" t="s">
         <v>269</v>
+      </c>
+      <c r="L38" s="15">
+        <v>5.21</v>
+      </c>
+      <c r="M38">
+        <v>647.99526000000003</v>
+      </c>
+      <c r="N38">
+        <f>(F38-M38)/M38*10^6</f>
+        <v>-0.57407827347991991</v>
       </c>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
@@ -20568,7 +20648,7 @@
         <v>697.99170500000002</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5759499814660644E-2</v>
       </c>
       <c r="F39">
@@ -20582,6 +20662,16 @@
       </c>
       <c r="K39" s="8" t="s">
         <v>245</v>
+      </c>
+      <c r="L39" s="15">
+        <v>5.65</v>
+      </c>
+      <c r="M39">
+        <v>697.99181999999996</v>
+      </c>
+      <c r="N39">
+        <f>(F39-M39)/M39*10^6</f>
+        <v>-0.18051787470697617</v>
       </c>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
@@ -20609,7 +20699,7 @@
         <v>747.98889499999996</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.52808298511570106</v>
       </c>
       <c r="F40">
@@ -20623,6 +20713,16 @@
       </c>
       <c r="K40" s="8" t="s">
         <v>159</v>
+      </c>
+      <c r="L40" s="15">
+        <v>6.05</v>
+      </c>
+      <c r="M40">
+        <v>747.98991000000001</v>
+      </c>
+      <c r="N40">
+        <f>(F40-M40)/M40*10^6</f>
+        <v>-1.8850521659635544</v>
       </c>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
@@ -20648,7 +20748,7 @@
         <v>847.98320000000001</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2830459329094293</v>
       </c>
       <c r="F41">

</xml_diff>

<commit_message>
new suspect data for semi quant
</commit_message>
<xml_diff>
--- a/data/Sus. + ms2 data.xlsx
+++ b/data/Sus. + ms2 data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Labuser\Documents\GitHub\PFOA_semi_quant\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B398A68-328D-4264-BF7F-197E9AA0224A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4EE5F4-8CFB-4B96-923C-FBD4808E2187}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="5790" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3900" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3902" uniqueCount="466">
   <si>
     <t>10_2 FTSA</t>
   </si>
@@ -1434,7 +1434,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1575,7 +1575,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18870,9 +18870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19587,6 +19587,9 @@
       <c r="H12" t="s">
         <v>371</v>
       </c>
+      <c r="I12" s="15" t="s">
+        <v>434</v>
+      </c>
       <c r="J12">
         <v>3.8</v>
       </c>
@@ -19647,6 +19650,9 @@
       </c>
       <c r="H13" t="s">
         <v>380</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>434</v>
       </c>
       <c r="J13">
         <v>4.8150000000000004</v>

</xml_diff>

<commit_message>
last minute figure changes
</commit_message>
<xml_diff>
--- a/data/Sus. + ms2 data.xlsx
+++ b/data/Sus. + ms2 data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Labuser\Documents\GitHub\PFOA_semi_quant\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4EE5F4-8CFB-4B96-923C-FBD4808E2187}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623B00BE-898A-462F-8715-F349AC60E228}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="5790" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18870,9 +18870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>